<commit_message>
fix error in GPT-4 prices
</commit_message>
<xml_diff>
--- a/openai_api.xlsx
+++ b/openai_api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reza/Desktop/OpenAI-API-Sum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E29AC5A-FE66-D74B-BB64-791C541BE6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D084626B-C7A5-2B41-8BB1-29F509A783D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{67FD31E5-A99B-2141-B049-787CE3700865}"/>
   </bookViews>
@@ -304,14 +304,6 @@
     <t>0.0200</t>
   </si>
   <si>
-    <t>0.0600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.1200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>InstructGPT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -528,6 +520,14 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>I: 0.0300
+O: 0.0600</t>
+  </si>
+  <si>
+    <t>I: 0.0600
+O: 0.1200</t>
   </si>
 </sst>
 </file>
@@ -797,6 +797,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -823,9 +826,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863BC0F5-2438-DE40-AAD1-CCDF4F247BF4}">
   <dimension ref="A3:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1168,48 +1168,48 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10">
-      <c r="A3" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
+      <c r="A3" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="1:10" ht="66">
-      <c r="A6" s="23" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+    </row>
+    <row r="6" spans="1:10" ht="44">
+      <c r="A6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>7</v>
@@ -1236,10 +1236,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="21">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="5" t="s">
         <v>35</v>
       </c>
@@ -1266,8 +1266,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="21">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
@@ -1294,8 +1294,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="21">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="5" t="s">
         <v>37</v>
       </c>
@@ -1322,8 +1322,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="21">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="5" t="s">
         <v>38</v>
       </c>
@@ -1350,10 +1350,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="36">
-      <c r="A11" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -1378,12 +1378,12 @@
         <v>46</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="22">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="22">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="6" t="s">
         <v>15</v>
       </c>
@@ -1434,12 +1434,12 @@
         <v>46</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="22">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
@@ -1462,12 +1462,12 @@
         <v>46</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
@@ -1490,12 +1490,12 @@
         <v>46</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="38" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1520,12 +1520,12 @@
         <v>46</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="49" customHeight="1">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="6" t="s">
         <v>21</v>
       </c>
@@ -1548,16 +1548,16 @@
         <v>46</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="22">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>17</v>
@@ -1578,20 +1578,20 @@
         <v>47</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="54">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>77</v>
+        <v>64</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="F19" s="9">
         <v>4096</v>
@@ -1606,20 +1606,20 @@
         <v>47</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="36">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="28" t="s">
-        <v>77</v>
+      <c r="E20" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="F20" s="9">
         <v>4096</v>
@@ -1638,16 +1638,16 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="36">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>78</v>
+        <v>64</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>76</v>
       </c>
       <c r="F21" s="9">
         <v>16384</v>
@@ -1662,22 +1662,22 @@
         <v>47</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="22">
-      <c r="A22" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="36">
+      <c r="A22" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>58</v>
+      <c r="E22" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="F22" s="9">
         <v>8192</v>
@@ -1695,17 +1695,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="22">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
+    <row r="23" spans="1:10" ht="36">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="F23" s="9">
         <v>8192</v>
@@ -1720,20 +1720,20 @@
         <v>47</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="22">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="36">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>58</v>
+      <c r="E24" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="F24" s="9">
         <v>8192</v>
@@ -1751,17 +1751,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="72">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
+    <row r="25" spans="1:10" ht="36">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>59</v>
+      <c r="E25" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="F25" s="9">
         <v>32768</v>
@@ -1776,20 +1776,20 @@
         <v>47</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="22">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="36">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="F26" s="9">
         <v>32768</v>
@@ -1804,20 +1804,20 @@
         <v>47</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="54">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="36">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>59</v>
+      <c r="E27" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="F27" s="9">
         <v>32768</v>
@@ -1832,7 +1832,7 @@
         <v>47</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>